<commit_message>
[modoo] subpage 추가 및 main 스크립트 수정, xlsx 수정
</commit_message>
<xml_diff>
--- a/langchain/src/openai/modoo/matching_block_data/Modoo_matching_blocks.xlsx
+++ b/langchain/src/openai/modoo/matching_block_data/Modoo_matching_blocks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\COM\VscodeProject\LLM_RAG_TEST\langchain\src\openai\modoo\matching_block_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C333612D-BE1D-4083-8AA6-DAED9308F6C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48352197-4224-406C-B9C2-33E2CD9B613D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{A840D17A-F1F4-4053-87B5-54732BB4FD71}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{A840D17A-F1F4-4053-87B5-54732BB4FD71}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="88">
   <si>
     <t>block_id</t>
   </si>
@@ -279,13 +279,6 @@
     <t>{
 "h5_0": "10",
 "h2_0": "15",
-"p_0": "100"
-}</t>
-  </si>
-  <si>
-    <t>{
-"h5_0": "10",
-"h2_0": "15",
 "h4_0": "10",
 "p_0": "100"
 }</t>
@@ -536,6 +529,18 @@
 }
 ]
 }</t>
+  </si>
+  <si>
+    <t>{
+"h5_0": "10",
+"h2_0": "15",
+"p_0": "100"
+}</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>h5_h2_p_img*4</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -961,8 +966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4994A09-5628-4C1B-827A-1AF11AFEE91F}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D31"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1037,7 +1042,7 @@
         <v>12</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>10</v>
@@ -1051,7 +1056,7 @@
         <v>14</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>15</v>
@@ -1079,7 +1084,7 @@
         <v>17</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>10</v>
@@ -1093,7 +1098,7 @@
         <v>20</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>21</v>
@@ -1107,7 +1112,7 @@
         <v>6</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>7</v>
@@ -1121,7 +1126,7 @@
         <v>24</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>25</v>
@@ -1135,7 +1140,7 @@
         <v>27</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>28</v>
@@ -1149,7 +1154,7 @@
         <v>30</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>31</v>
@@ -1163,7 +1168,7 @@
         <v>33</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>34</v>
@@ -1177,7 +1182,7 @@
         <v>30</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>31</v>
@@ -1191,7 +1196,7 @@
         <v>33</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>34</v>
@@ -1205,7 +1210,7 @@
         <v>33</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>34</v>
@@ -1219,7 +1224,7 @@
         <v>39</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>40</v>
@@ -1233,7 +1238,7 @@
         <v>42</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>43</v>
@@ -1247,7 +1252,7 @@
         <v>45</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>46</v>
@@ -1261,7 +1266,7 @@
         <v>27</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>28</v>
@@ -1275,7 +1280,7 @@
         <v>49</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>10</v>
@@ -1289,7 +1294,7 @@
         <v>17</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>10</v>
@@ -1300,10 +1305,10 @@
         <v>51</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>12</v>
+        <v>87</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>10</v>
@@ -1317,7 +1322,7 @@
         <v>53</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>10</v>
@@ -1331,7 +1336,7 @@
         <v>55</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>10</v>
@@ -1339,7 +1344,7 @@
     </row>
     <row r="27" spans="1:4" ht="64.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>57</v>
@@ -1359,7 +1364,7 @@
         <v>57</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>10</v>
@@ -1373,7 +1378,7 @@
         <v>59</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>60</v>
@@ -1401,7 +1406,7 @@
         <v>64</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>65</v>

</xml_diff>